<commit_message>
RNN - Testes, já com evaluate
</commit_message>
<xml_diff>
--- a/Desafios-NLP/2021-02-Sentimentos-Twitter/Resultados.xlsx
+++ b/Desafios-NLP/2021-02-Sentimentos-Twitter/Resultados.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\Cursos\Pos-BI-Master\Desafio NLP\Desafio 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bi-master\Desafios-NLP\2021-02-Sentimentos-Twitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDB16AF-4794-4507-A342-545013883FED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D50A7A8-22B3-4780-AFC0-732DFC141D51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BC61AAF2-52F3-461E-89E6-B3D31226DBB8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{BC61AAF2-52F3-461E-89E6-B3D31226DBB8}"/>
   </bookViews>
   <sheets>
-    <sheet name="3 Labels" sheetId="1" r:id="rId1"/>
+    <sheet name="Machine Learning" sheetId="1" r:id="rId1"/>
+    <sheet name="Recurrent Neural Network" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="36">
   <si>
     <t>Tokenizer</t>
   </si>
@@ -97,13 +98,58 @@
   </si>
   <si>
     <t>Não</t>
+  </si>
+  <si>
+    <t>Tipo LSTM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Padding</t>
+  </si>
+  <si>
+    <t>Acurácia</t>
+  </si>
+  <si>
+    <t>Acurácia Validação</t>
+  </si>
+  <si>
+    <t>&lt;unknown&gt;</t>
+  </si>
+  <si>
+    <t>Tamanho Sentença</t>
+  </si>
+  <si>
+    <t>Labels Agrupados</t>
+  </si>
+  <si>
+    <t># --&gt; &lt;hashtag&gt;</t>
+  </si>
+  <si>
+    <t>Agrupar Labels</t>
+  </si>
+  <si>
+    <t>Epochs</t>
+  </si>
+  <si>
+    <t>Batch Size</t>
+  </si>
+  <si>
+    <t>Acurácia Teste</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>LSTM somente</t>
+  </si>
+  <si>
+    <t>Bidirecional somente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +160,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -173,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -195,6 +249,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,71 +576,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6853B0C-EF2B-4306-B2F3-118C39CCEC30}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.734375" customWidth="1"/>
-    <col min="2" max="2" width="13.1015625" customWidth="1"/>
-    <col min="3" max="3" width="12.47265625" customWidth="1"/>
-    <col min="4" max="4" width="20.26171875" customWidth="1"/>
-    <col min="5" max="5" width="11.5234375" customWidth="1"/>
-    <col min="6" max="6" width="13.47265625" customWidth="1"/>
-    <col min="8" max="8" width="9.89453125" customWidth="1"/>
-    <col min="9" max="9" width="14.578125" customWidth="1"/>
-    <col min="10" max="10" width="13.26171875" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="29.3671875" customWidth="1"/>
+    <col min="1" max="1" width="18" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
+    <row r="2" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -583,66 +653,72 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H2" s="1">
         <v>20</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>2</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>80</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="4">
+      <c r="K2" s="1"/>
+      <c r="L2" s="4">
         <v>77.5</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G3" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H3" s="1">
         <v>20</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>2</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>80</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="3">
+      <c r="K3" s="1"/>
+      <c r="L3" s="3">
         <v>77</v>
       </c>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -651,100 +727,109 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G4" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H4" s="1">
         <v>1E-3</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>3</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>78.5</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="3">
+      <c r="K4" s="1"/>
+      <c r="L4" s="3">
         <v>77</v>
       </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G5" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H5" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>3</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>68.400000000000006</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="3">
+      <c r="K5" s="1"/>
+      <c r="L5" s="3">
         <v>68.2</v>
       </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.8</v>
+        <v>10</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="G6" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H6" s="1">
         <v>1E-3</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>3</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>77.98</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="3">
+      <c r="K6" s="1"/>
+      <c r="L6" s="3">
         <v>67.2</v>
       </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -755,32 +840,35 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1">
-        <v>0.8</v>
+      <c r="F7" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="G7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H7" s="1">
         <v>1E-3</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>3</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>78.5</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="3">
+      <c r="K7" s="1"/>
+      <c r="L7" s="3">
         <v>73.8</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
+    <row r="8" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -789,194 +877,212 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="1">
         <v>20</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>3</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>80.099999999999994</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
+      <c r="K8" s="1"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H9" s="1">
         <v>20</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>3</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>80.2</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
+      <c r="K9" s="1"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G10" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H10" s="1">
         <v>20</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>1</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>80.7</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
+      <c r="K10" s="1"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H11" s="1">
         <v>20</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>1</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>80.7</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="4" t="s">
-        <v>6</v>
+      <c r="L11" s="3"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="G12" s="4">
-        <v>10</v>
+        <v>0.8</v>
       </c>
       <c r="H12" s="4">
+        <v>10</v>
+      </c>
+      <c r="I12" s="4">
         <v>1</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="4">
         <v>81.349999999999994</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="3">
+      <c r="K12" s="1"/>
+      <c r="L12" s="3">
         <v>77.28</v>
       </c>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1" t="s">
-        <v>6</v>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0.8</v>
+      <c r="F13" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G13" s="1">
-        <v>10</v>
+        <v>0.8</v>
       </c>
       <c r="H13" s="1">
+        <v>10</v>
+      </c>
+      <c r="I13" s="1">
         <v>1</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>81.17</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
+      <c r="K13" s="1"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -985,126 +1091,138 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G14" s="1">
-        <v>10</v>
+        <v>0.8</v>
       </c>
       <c r="H14" s="1">
+        <v>10</v>
+      </c>
+      <c r="I14" s="1">
         <v>1</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>81.06</v>
       </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="1" t="s">
-        <v>6</v>
+      <c r="K14" s="1"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="G15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>1</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>80.900000000000006</v>
       </c>
-      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="1" t="s">
-        <v>6</v>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G16" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H16" s="1">
         <v>5</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>80.900000000000006</v>
       </c>
-      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="1" t="s">
-        <v>6</v>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G17" s="1">
-        <v>10</v>
+        <v>0.8</v>
       </c>
       <c r="H17" s="1">
+        <v>10</v>
+      </c>
+      <c r="I17" s="1">
         <v>3</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>80.7</v>
       </c>
-      <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="1" t="s">
-        <v>6</v>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
@@ -1113,126 +1231,138 @@
         <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G18" s="1">
-        <v>10</v>
+        <v>0.8</v>
       </c>
       <c r="H18" s="1">
+        <v>10</v>
+      </c>
+      <c r="I18" s="1">
         <v>1</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>81</v>
       </c>
-      <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="1" t="s">
-        <v>6</v>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G19" s="1">
-        <v>10</v>
+        <v>0.8</v>
       </c>
       <c r="H19" s="1">
+        <v>10</v>
+      </c>
+      <c r="I19" s="1">
         <v>1</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <v>79.7</v>
       </c>
-      <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G20" s="1">
-        <v>10</v>
+        <v>0.8</v>
       </c>
       <c r="H20" s="1">
+        <v>10</v>
+      </c>
+      <c r="I20" s="1">
         <v>1</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>79.7</v>
       </c>
-      <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="1" t="s">
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0.8</v>
+        <v>7</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G21" s="1">
-        <v>10</v>
+        <v>0.8</v>
       </c>
       <c r="H21" s="1">
+        <v>10</v>
+      </c>
+      <c r="I21" s="1">
         <v>1</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <v>79.5</v>
       </c>
-      <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="1" t="s">
-        <v>6</v>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -1241,28 +1371,33 @@
         <v>18</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0.8</v>
+        <v>18</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="G22" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H22" s="1">
         <v>1E-3</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>1</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <v>78.400000000000006</v>
       </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1">
+      <c r="K22" s="1"/>
+      <c r="L22" s="1">
         <v>76.430000000000007</v>
       </c>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="1"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1274,6 +1409,263 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FEFB37-A6B4-48CA-B2ED-0A6E3AD82751}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="23.140625" style="8"/>
+    <col min="4" max="4" width="21" style="8" customWidth="1"/>
+    <col min="5" max="10" width="23.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8">
+        <v>85.81</v>
+      </c>
+      <c r="H2" s="8">
+        <v>82.45</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8">
+        <v>50</v>
+      </c>
+      <c r="C3" s="8">
+        <v>32</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="8">
+        <v>89.31</v>
+      </c>
+      <c r="H3" s="8">
+        <v>83.81</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8">
+        <v>40</v>
+      </c>
+      <c r="C4" s="8">
+        <v>32</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="8">
+        <v>89.32</v>
+      </c>
+      <c r="H4" s="8">
+        <v>83.22</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="8">
+        <v>40</v>
+      </c>
+      <c r="C5" s="8">
+        <v>32</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8">
+        <v>40</v>
+      </c>
+      <c r="C6" s="8">
+        <v>32</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="8">
+        <v>91.01</v>
+      </c>
+      <c r="H6" s="8">
+        <v>80.73</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8">
+        <v>40</v>
+      </c>
+      <c r="C7" s="8">
+        <v>64</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="8">
+        <v>87.28</v>
+      </c>
+      <c r="H7" s="8">
+        <v>81.569999999999993</v>
+      </c>
+      <c r="I7" s="8">
+        <v>80.3</v>
+      </c>
+      <c r="J7" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <v>40</v>
+      </c>
+      <c r="C8" s="8">
+        <v>32</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>